<commit_message>
Update BOM file with new changes.
Binary files differ.
</commit_message>
<xml_diff>
--- a/Hutschienenmoped-XL_2ETH/Sample-BOM_JLCSMT.xlsx
+++ b/Hutschienenmoped-XL_2ETH/Sample-BOM_JLCSMT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ms\ISOBUS_Hardware\Hutschienenmoped-XL_2ETH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFDE136-D67D-48E4-83BE-9E62C9B4BB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7BEE23-37D3-4316-AEEE-48E34EE25109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41805" yWindow="1230" windowWidth="33435" windowHeight="18735" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5385" yWindow="2265" windowWidth="33435" windowHeight="18735" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="80">
   <si>
     <t>Comment</t>
   </si>
@@ -268,6 +268,33 @@
   </si>
   <si>
     <t>TLE9250VSJ</t>
+  </si>
+  <si>
+    <t>61300421121</t>
+  </si>
+  <si>
+    <t>61300615721</t>
+  </si>
+  <si>
+    <t>61301015721</t>
+  </si>
+  <si>
+    <t>61302211821</t>
+  </si>
+  <si>
+    <t>638207222005</t>
+  </si>
+  <si>
+    <t>638207222007</t>
+  </si>
+  <si>
+    <t>638207222008</t>
+  </si>
+  <si>
+    <t>645004114822</t>
+  </si>
+  <si>
+    <t>61300621121</t>
   </si>
 </sst>
 </file>
@@ -344,7 +371,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -364,6 +391,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -710,13 +738,13 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A33"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="26" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.375" customWidth="1"/>
+    <col min="2" max="2" width="80.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.125" customWidth="1"/>
     <col min="4" max="4" width="24.5" customWidth="1"/>
   </cols>
@@ -740,8 +768,8 @@
       <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6">
-        <v>61300621121</v>
+      <c r="C2" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="D2" s="5"/>
     </row>
@@ -766,85 +794,88 @@
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="6">
-        <v>61300421121</v>
+      <c r="A5" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6">
-        <v>61300421121</v>
+      <c r="C5" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="6">
-        <v>61300615721</v>
+      <c r="A6" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6">
-        <v>61300615721</v>
+      <c r="C6" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="6">
-        <v>61301015721</v>
+      <c r="A7" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6">
-        <v>61301015721</v>
+      <c r="C7" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="6">
-        <v>61302211821</v>
+      <c r="A8" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="6">
-        <v>61302211821</v>
+      <c r="C8" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="6">
-        <v>638207222005</v>
+      <c r="A9" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="6">
-        <v>638207222005</v>
-      </c>
+      <c r="C9" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="6">
-        <v>638207222007</v>
+      <c r="A10" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="6">
-        <v>638207222007</v>
-      </c>
+      <c r="C10" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="6">
-        <v>638207222008</v>
+      <c r="A11" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="6">
-        <v>638207222008</v>
-      </c>
+      <c r="C11" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="6" t="s">
@@ -856,6 +887,7 @@
       <c r="C12" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="6" t="s">
@@ -867,6 +899,7 @@
       <c r="C13" s="6" t="s">
         <v>39</v>
       </c>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="6" t="s">
@@ -878,6 +911,7 @@
       <c r="C14" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="6" t="s">
@@ -889,6 +923,7 @@
       <c r="C15" s="6" t="s">
         <v>40</v>
       </c>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="6" t="s">
@@ -900,8 +935,9 @@
       <c r="C16" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="6" t="s">
         <v>56</v>
       </c>
@@ -911,8 +947,9 @@
       <c r="C17" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A18" s="6" t="s">
         <v>57</v>
       </c>
@@ -922,8 +959,9 @@
       <c r="C18" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="6" t="s">
         <v>57</v>
       </c>
@@ -933,8 +971,9 @@
       <c r="C19" s="6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="6" t="s">
         <v>58</v>
       </c>
@@ -944,8 +983,9 @@
       <c r="C20" s="6" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A21" s="6" t="s">
         <v>59</v>
       </c>
@@ -955,8 +995,9 @@
       <c r="C21" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A22" s="6" t="s">
         <v>60</v>
       </c>
@@ -966,8 +1007,9 @@
       <c r="C22" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A23" s="6" t="s">
         <v>61</v>
       </c>
@@ -977,8 +1019,9 @@
       <c r="C23" s="6" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A24" s="6" t="s">
         <v>62</v>
       </c>
@@ -988,8 +1031,9 @@
       <c r="C24" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="6" t="s">
         <v>63</v>
       </c>
@@ -999,8 +1043,9 @@
       <c r="C25" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="D25" s="5"/>
+    </row>
+    <row r="26" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="6" t="s">
         <v>64</v>
       </c>
@@ -1010,8 +1055,9 @@
       <c r="C26" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="6" t="s">
         <v>65</v>
       </c>
@@ -1021,8 +1067,9 @@
       <c r="C27" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="D27" s="5"/>
+    </row>
+    <row r="28" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="6" t="s">
         <v>66</v>
       </c>
@@ -1032,8 +1079,9 @@
       <c r="C28" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A29" s="6" t="s">
         <v>67</v>
       </c>
@@ -1043,19 +1091,21 @@
       <c r="C29" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="20.100000000000001" customHeight="1">
-      <c r="A30" s="6">
-        <v>645004114822</v>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A30" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="6">
-        <v>645004114822</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="C30" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="6" t="s">
         <v>68</v>
       </c>
@@ -1065,8 +1115,9 @@
       <c r="C31" s="6" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A32" s="6" t="s">
         <v>69</v>
       </c>
@@ -1076,8 +1127,9 @@
       <c r="C32" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="20.100000000000001" customHeight="1">
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="6" t="s">
         <v>70</v>
       </c>
@@ -1087,6 +1139,7 @@
       <c r="C33" s="6" t="s">
         <v>51</v>
       </c>
+      <c r="D33" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>